<commit_message>
modifica nome variabile (prefisso "diagnosticDB")+ modifiche minori a gen skid pems aux
</commit_message>
<xml_diff>
--- a/template_excel/template_HVAC_HH.xlsx
+++ b/template_excel/template_HVAC_HH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhoaenergy.sharepoint.com/sites/Q1043-HyESScontainerHDevolution/Documenti condivisi/General/08_SW standardization/11_Alarms_Template/Alarms_automation_HH/template_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{A14F61D2-7CB4-46D1-9027-F749AD58FD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CCC2036-7806-4621-BB78-608B61824191}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{A14F61D2-7CB4-46D1-9027-F749AD58FD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9DB8019-D1E7-4426-9096-CA267D36BB0F}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ACAA2209-6B97-4E62-84C4-F3D4F647F045}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3120" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3120" uniqueCount="108">
   <si>
     <t/>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>W |Code 068: Cooling fan controller fault | HVAC</t>
-  </si>
-  <si>
-    <t>W |Spare | HVAC</t>
   </si>
   <si>
     <t>A |Code 011: Forced shut-down | HVAC</t>
@@ -303,17 +300,83 @@
     <t>A |Code 111: Humidity probe return error | HVAC</t>
   </si>
   <si>
-    <t>A |Spare | HVAC</t>
+    <t>A |Spare wAlarm4.2 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.3 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.4 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.5 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.6 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.7 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.8 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.9 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.10 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.11 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.12 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.13 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.14 | HVAC</t>
+  </si>
+  <si>
+    <t>A |Spare wAlarm4.15 | HVAC</t>
+  </si>
+  <si>
+    <t>W |Spare wWarning.9 | HVAC</t>
+  </si>
+  <si>
+    <t>W |Spare  wWarning.15 | HVAC</t>
+  </si>
+  <si>
+    <t>W |Spare wWarning.14 | HVAC</t>
+  </si>
+  <si>
+    <t>W |Spare wWarning.13 | HVAC</t>
+  </si>
+  <si>
+    <t>W |Spare wWarning.12 | HVAC</t>
+  </si>
+  <si>
+    <t>W |Spare wWarning.11 | HVAC</t>
+  </si>
+  <si>
+    <t>W |Spare wWarning.10 | HVAC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -664,7 +727,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6160FB5D-CE7F-49AE-B791-39BCA4E55F21}">
   <dimension ref="A1:AS80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1934,7 +1999,7 @@
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -2071,7 +2136,7 @@
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -2208,7 +2273,7 @@
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -2345,7 +2410,7 @@
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -2482,7 +2547,7 @@
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -2619,7 +2684,7 @@
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -2756,7 +2821,7 @@
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -2893,7 +2958,7 @@
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -3030,7 +3095,7 @@
     </row>
     <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -3167,7 +3232,7 @@
     </row>
     <row r="19" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -3304,7 +3369,7 @@
     </row>
     <row r="20" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -3441,7 +3506,7 @@
     </row>
     <row r="21" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -3578,7 +3643,7 @@
     </row>
     <row r="22" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -3715,7 +3780,7 @@
     </row>
     <row r="23" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -3852,7 +3917,7 @@
     </row>
     <row r="24" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -3989,7 +4054,7 @@
     </row>
     <row r="25" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -4126,7 +4191,7 @@
     </row>
     <row r="26" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -4263,7 +4328,7 @@
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -4400,7 +4465,7 @@
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -4537,7 +4602,7 @@
     </row>
     <row r="29" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -4674,7 +4739,7 @@
     </row>
     <row r="30" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -4811,7 +4876,7 @@
     </row>
     <row r="31" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -4948,7 +5013,7 @@
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -5085,7 +5150,7 @@
     </row>
     <row r="33" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -5222,7 +5287,7 @@
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -5359,7 +5424,7 @@
     </row>
     <row r="35" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -5496,7 +5561,7 @@
     </row>
     <row r="36" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
@@ -5633,7 +5698,7 @@
     </row>
     <row r="37" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
@@ -5770,7 +5835,7 @@
     </row>
     <row r="38" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -5907,7 +5972,7 @@
     </row>
     <row r="39" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -6044,7 +6109,7 @@
     </row>
     <row r="40" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
@@ -6181,7 +6246,7 @@
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
         <v>6</v>
@@ -6318,7 +6383,7 @@
     </row>
     <row r="42" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
@@ -6455,7 +6520,7 @@
     </row>
     <row r="43" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
         <v>6</v>
@@ -6592,7 +6657,7 @@
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44" t="s">
         <v>6</v>
@@ -6729,7 +6794,7 @@
     </row>
     <row r="45" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45" t="s">
         <v>6</v>
@@ -6866,7 +6931,7 @@
     </row>
     <row r="46" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B46" t="s">
         <v>6</v>
@@ -7003,7 +7068,7 @@
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
@@ -7140,7 +7205,7 @@
     </row>
     <row r="48" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
         <v>6</v>
@@ -7277,7 +7342,7 @@
     </row>
     <row r="49" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
         <v>6</v>
@@ -7414,7 +7479,7 @@
     </row>
     <row r="50" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
@@ -7551,7 +7616,7 @@
     </row>
     <row r="51" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
@@ -7688,7 +7753,7 @@
     </row>
     <row r="52" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
@@ -7825,7 +7890,7 @@
     </row>
     <row r="53" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B53" t="s">
         <v>6</v>
@@ -7962,7 +8027,7 @@
     </row>
     <row r="54" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
         <v>6</v>
@@ -8099,7 +8164,7 @@
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B55" t="s">
         <v>6</v>
@@ -8236,7 +8301,7 @@
     </row>
     <row r="56" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
@@ -8373,7 +8438,7 @@
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B57" t="s">
         <v>6</v>
@@ -8510,7 +8575,7 @@
     </row>
     <row r="58" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
@@ -8647,7 +8712,7 @@
     </row>
     <row r="59" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
@@ -8784,7 +8849,7 @@
     </row>
     <row r="60" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B60" t="s">
         <v>6</v>
@@ -8921,7 +8986,7 @@
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B61" t="s">
         <v>6</v>
@@ -9058,7 +9123,7 @@
     </row>
     <row r="62" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B62" t="s">
         <v>6</v>
@@ -9195,7 +9260,7 @@
     </row>
     <row r="63" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B63" t="s">
         <v>6</v>
@@ -9332,7 +9397,7 @@
     </row>
     <row r="64" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
@@ -9469,7 +9534,7 @@
     </row>
     <row r="65" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B65" t="s">
         <v>6</v>
@@ -9606,7 +9671,7 @@
     </row>
     <row r="66" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
@@ -9743,7 +9808,7 @@
     </row>
     <row r="67" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B67" t="s">
         <v>6</v>
@@ -10017,7 +10082,7 @@
     </row>
     <row r="69" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B69" t="s">
         <v>6</v>
@@ -10154,7 +10219,7 @@
     </row>
     <row r="70" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B70" t="s">
         <v>6</v>
@@ -10291,7 +10356,7 @@
     </row>
     <row r="71" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B71" t="s">
         <v>6</v>
@@ -10428,7 +10493,7 @@
     </row>
     <row r="72" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
@@ -10565,7 +10630,7 @@
     </row>
     <row r="73" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B73" t="s">
         <v>6</v>
@@ -10702,7 +10767,7 @@
     </row>
     <row r="74" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
@@ -10839,7 +10904,7 @@
     </row>
     <row r="75" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
@@ -10976,7 +11041,7 @@
     </row>
     <row r="76" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B76" t="s">
         <v>6</v>
@@ -11113,7 +11178,7 @@
     </row>
     <row r="77" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
@@ -11250,7 +11315,7 @@
     </row>
     <row r="78" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B78" t="s">
         <v>6</v>
@@ -11387,7 +11452,7 @@
     </row>
     <row r="79" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B79" t="s">
         <v>6</v>
@@ -11524,7 +11589,7 @@
     </row>
     <row r="80" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B80" t="s">
         <v>6</v>
@@ -11660,6 +11725,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>